<commit_message>
merged with the master
</commit_message>
<xml_diff>
--- a/to_do_eg/test.xlsx
+++ b/to_do_eg/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>ddd@example.com</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>ccc@example.com</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -446,9 +452,17 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -458,7 +472,8 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>